<commit_message>
add Students Detail.xlsx and StudentDetailsReader.java
</commit_message>
<xml_diff>
--- a/Students Detail.xlsx
+++ b/Students Detail.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83375B13-1045-436B-B8D0-11F3421F1E62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E49A74-5F4A-4644-A959-160975BF4170}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="shet61" r:id="rId5" sheetId="2"/>
+    <sheet name="sheet61" r:id="rId6" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="44">
   <si>
     <t>rollno</t>
   </si>
@@ -489,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>